<commit_message>
updating formulation 2 and 3 input files
</commit_message>
<xml_diff>
--- a/example/formulation_2/input/PySedSim_Input_File - Sambor_EA_formulation_2_deterministic_reeval.xlsx
+++ b/example/formulation_2/input/PySedSim_Input_File - Sambor_EA_formulation_2_deterministic_reeval.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr date1904="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="4860" yWindow="1980" windowWidth="7140" windowHeight="3585" tabRatio="848" firstSheet="6" activeTab="7"/>
+    <workbookView xWindow="4860" yWindow="2040" windowWidth="7140" windowHeight="3525" tabRatio="848" firstSheet="13" activeTab="20"/>
   </bookViews>
   <sheets>
     <sheet name="Simulation Specifications" sheetId="54" r:id="rId1"/>
@@ -20,22 +20,22 @@
     <sheet name="Tailwater Rating Curve" sheetId="80" r:id="rId11"/>
     <sheet name="DPS" sheetId="103" r:id="rId12"/>
     <sheet name="Optimization" sheetId="104" r:id="rId13"/>
-    <sheet name="Reevaluation" sheetId="112" r:id="rId14"/>
-    <sheet name="Max Reservoir WSE" sheetId="105" r:id="rId15"/>
-    <sheet name="Junction Flow Distribution" sheetId="90" r:id="rId16"/>
-    <sheet name="Reservoir Natural Bypass" sheetId="106" r:id="rId17"/>
-    <sheet name="Egg Passage Targets" sheetId="85" r:id="rId18"/>
-    <sheet name="Tradeoff Plotting" sheetId="117" r:id="rId19"/>
-    <sheet name="Parallel Axis Plotting" sheetId="115" r:id="rId20"/>
-    <sheet name="Export Preferences" sheetId="122" r:id="rId21"/>
+    <sheet name="Max Reservoir WSE" sheetId="105" r:id="rId14"/>
+    <sheet name="Junction Flow Distribution" sheetId="90" r:id="rId15"/>
+    <sheet name="Reservoir Natural Bypass" sheetId="106" r:id="rId16"/>
+    <sheet name="Egg Passage Targets" sheetId="85" r:id="rId17"/>
+    <sheet name="Tradeoff Plotting" sheetId="117" r:id="rId18"/>
+    <sheet name="Parallel Axis Plotting" sheetId="115" r:id="rId19"/>
+    <sheet name="Export Preferences" sheetId="122" r:id="rId20"/>
+    <sheet name="Reevaluation" sheetId="123" r:id="rId21"/>
   </sheets>
   <externalReferences>
     <externalReference r:id="rId22"/>
   </externalReferences>
   <definedNames>
-    <definedName name="IncSedLoadCalibrationOptions" localSheetId="13">[1]!Table1[Incremental Sediment Load Calibration Options]</definedName>
+    <definedName name="IncSedLoadCalibrationOptions" localSheetId="20">[1]!Table1[Incremental Sediment Load Calibration Options]</definedName>
     <definedName name="IncSedLoadCalibrationOptions">[1]!Table1[Incremental Sediment Load Calibration Options]</definedName>
-    <definedName name="Sediment_discharge_from_reaches__channels___calibration_preferences_for_determining_coefficient_a__in_aQb" localSheetId="13">[1]!Table2[[#All],[Sediment discharge from reaches (channels): calibration preferences for determining coefficient a (in aQb)]]</definedName>
+    <definedName name="Sediment_discharge_from_reaches__channels___calibration_preferences_for_determining_coefficient_a__in_aQb" localSheetId="20">[1]!Table2[[#All],[Sediment discharge from reaches (channels): calibration preferences for determining coefficient a (in aQb)]]</definedName>
     <definedName name="Sediment_discharge_from_reaches__channels___calibration_preferences_for_determining_coefficient_a__in_aQb">[1]!Table2[[#All],[Sediment discharge from reaches (channels): calibration preferences for determining coefficient a (in aQb)]]</definedName>
     <definedName name="solver_adj" localSheetId="4" hidden="1">'E-V-A-S'!#REF!</definedName>
     <definedName name="solver_cvg" localSheetId="4" hidden="1">0.0001</definedName>
@@ -70,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1109" uniqueCount="339">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1121" uniqueCount="343">
   <si>
     <t/>
   </si>
@@ -923,6 +923,9 @@
     <t>fraction inflow</t>
   </si>
   <si>
+    <t>Stochastic</t>
+  </si>
+  <si>
     <t>Maximum Wallclock Time to Run Optimization (hours)</t>
   </si>
   <si>
@@ -992,9 +995,6 @@
     <t>Borg runtime dynamics interval</t>
   </si>
   <si>
-    <t>Master-Slave</t>
-  </si>
-  <si>
     <t>D</t>
   </si>
   <si>
@@ -1421,71 +1421,84 @@
     <t>Hydropower_avg_MWH, water_surface_elevation, Q_in, Q_out, egg_pass, Q_out_under_thold, Q_out_over_thold, Hydropower_avg_MWH_over_thold, Hydropower_avg_MWH_under_thold, larv_surv_over_thold, larv_surv_under_thold, BS_W, capacity_active_reservoir, capacity_dead_reservoir, capacity_total_reservoir, res_flushed_load, SS_W_out, larv_mass_out_surv_total, Settled_mass</t>
   </si>
   <si>
+    <t>larv_pass_over_thold</t>
+  </si>
+  <si>
+    <t>larv_pass_under_thold</t>
+  </si>
+  <si>
     <t>Specify DPS policy</t>
   </si>
   <si>
+    <t>Bypass Flow (m^3 s^-1)</t>
+  </si>
+  <si>
+    <t>Bypass Flow - Dry (m^3 s^-1)</t>
+  </si>
+  <si>
+    <t>Bypass Flow - Dry</t>
+  </si>
+  <si>
+    <t>Bypass Flow - Wet (m^3 s^-1)</t>
+  </si>
+  <si>
+    <t>Bypass Flow - Wet</t>
+  </si>
+  <si>
+    <t>Larvae Flow Fraction</t>
+  </si>
+  <si>
     <t>larv_pass</t>
   </si>
   <si>
-    <t>larv_pass_over_thold</t>
-  </si>
-  <si>
-    <t>Larvae Flow Fraction</t>
-  </si>
-  <si>
     <t>Larvae Flow Fraction-Wet</t>
   </si>
   <si>
+    <t>Larvae Flow Fraction Wet</t>
+  </si>
+  <si>
     <t>Larvae Flow Fraction-Dry</t>
   </si>
   <si>
-    <t>larv_pass_under_thold</t>
-  </si>
-  <si>
-    <t>Larvae Flow Fraction Wet</t>
-  </si>
-  <si>
     <t>Larvae Flow Fraction Dry</t>
   </si>
   <si>
-    <t>Bypass Flow (m^3 s^-1)</t>
-  </si>
-  <si>
-    <t>Bypass Flow - Dry (m^3 s^-1)</t>
-  </si>
-  <si>
-    <t>Bypass Flow - Wet (m^3 s^-1)</t>
-  </si>
-  <si>
-    <t>Bypass Flow - Dry</t>
-  </si>
-  <si>
-    <t>Bypass Flow - Wet</t>
+    <t>Dry Season Daily Bypass \n Attraction Flow (m^3/s)</t>
+  </si>
+  <si>
+    <t>Dry Season \n Daily Bypass \n Attraction Flow \n (m^3/s)</t>
+  </si>
+  <si>
+    <t>177, 147, 103</t>
+  </si>
+  <si>
+    <t>Energy, Compromise, Larvae</t>
+  </si>
+  <si>
+    <t>Sambor EA</t>
+  </si>
+  <si>
+    <t>Sambor EA, Bypass Channel 1, Stung_Treng, Junction 4</t>
+  </si>
+  <si>
+    <t>Serial</t>
+  </si>
+  <si>
+    <t>77, 22, 86, 21</t>
   </si>
   <si>
     <t>52, 22, 18, 42</t>
-  </si>
-  <si>
-    <t>77, 22, 86, 21</t>
-  </si>
-  <si>
-    <t>Stochastic</t>
-  </si>
-  <si>
-    <t>Sambor EA</t>
-  </si>
-  <si>
-    <t>Sambor EA, Bypass Channel 1, Stung_Treng, Junction 4</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="#,##0.000"/>
     <numFmt numFmtId="166" formatCode="#,##0.0"/>
+    <numFmt numFmtId="167" formatCode="0.0000E+00"/>
   </numFmts>
   <fonts count="74" x14ac:knownFonts="1">
     <font>
@@ -4886,16 +4899,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="81" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="73" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="167" fontId="73" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="11" xfId="57" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="81" applyFont="1"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="10" xfId="57" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="11" xfId="57" applyBorder="1"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -7030,112 +7043,6 @@
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>581024</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>514349</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="TextBox 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0F00-000002000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="4914899" y="514350"/>
-          <a:ext cx="6105525" cy="2514600"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="lt1"/>
-        </a:solidFill>
-        <a:ln w="9525" cmpd="sng">
-          <a:solidFill>
-            <a:schemeClr val="lt1">
-              <a:shade val="50000"/>
-            </a:schemeClr>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100"/>
-            <a:t>Here's how I got this:</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="en-US" sz="1100"/>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100"/>
-            <a:t>Organized</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" baseline="0"/>
-            <a:t> Robert's outputs by flow, so we see the fraction into the reservoir versus total upstream flow versus elevation.</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="en-US" sz="1100" baseline="0"/>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" baseline="0"/>
-            <a:t>Then, I figured out the TERMINAL (max WSE) point for each flow. That is, the highest the reservoir water level  can get for a given flow. This plots that for every flow. Roberts methods differed for main stem flows above 17,086, so I simply used the trend for the highest flow values to predict the TERMINAL points for the higher flows, which quickly reach 40 masl.</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="en-US" sz="1100" baseline="0"/>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" baseline="0"/>
-            <a:t>Having done all of that, I then multiplied the total upstream flows by the terminal fraction, so they represent the RESERVOIR inflows, which are needed to be placed in the table here. The terminal fractions of reservoir inflow for high water levels become constant at about 46% at very high flows. (half of the water is getting into the anabranch). Is this a believable percentage? Need to check on this.</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
@@ -7482,7 +7389,7 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -7519,7 +7426,7 @@
         <v>62</v>
       </c>
       <c r="B4" s="53">
-        <v>41273</v>
+        <v>38716</v>
       </c>
       <c r="C4" s="79"/>
       <c r="D4" s="79"/>
@@ -7529,7 +7436,7 @@
         <v>113</v>
       </c>
       <c r="B5" s="53" t="s">
-        <v>336</v>
+        <v>154</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -7537,7 +7444,7 @@
         <v>112</v>
       </c>
       <c r="B6" s="83">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -7560,9 +7467,7 @@
   </sheetPr>
   <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -7579,7 +7484,7 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="49" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="B1" s="49"/>
       <c r="C1" s="49"/>
@@ -7648,9 +7553,7 @@
   </sheetPr>
   <dimension ref="A1:G29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -7660,7 +7563,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="128" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="B1" s="127"/>
     </row>
@@ -7876,7 +7779,7 @@
   <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A37" sqref="A37"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -7923,7 +7826,7 @@
         <v>3</v>
       </c>
       <c r="C2" s="85" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="D2" s="35">
         <v>21</v>
@@ -7949,7 +7852,7 @@
         <v>4</v>
       </c>
       <c r="C3" s="85" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="D3" s="35">
         <v>1</v>
@@ -7997,10 +7900,10 @@
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet18"/>
-  <dimension ref="A1:O25"/>
+  <dimension ref="A1:O27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -8011,7 +7914,7 @@
     <col min="4" max="5" width="11.875" style="127" customWidth="1"/>
     <col min="6" max="6" width="10.125" style="93" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.625" style="93" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.25" style="93" customWidth="1"/>
+    <col min="8" max="8" width="11.75" style="93" customWidth="1"/>
     <col min="9" max="9" width="19.625" style="93" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="11.875" style="93" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="12.25" style="93" customWidth="1"/>
@@ -8053,7 +7956,7 @@
         <v>129</v>
       </c>
       <c r="B5" s="48" t="s">
-        <v>177</v>
+        <v>340</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.2">
@@ -8069,7 +7972,7 @@
         <v>141</v>
       </c>
       <c r="B7" s="13">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.2">
@@ -8080,13 +7983,13 @@
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9" s="109" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B9" s="13"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10" s="109" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B10" s="107" t="s">
         <v>20</v>
@@ -8094,7 +7997,7 @@
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11" s="145" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B11" s="107" t="s">
         <v>20</v>
@@ -8102,7 +8005,7 @@
     </row>
     <row r="12" spans="1:15" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A12" s="146" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B12" s="107" t="s">
         <v>20</v>
@@ -8110,7 +8013,7 @@
     </row>
     <row r="13" spans="1:15" s="127" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A13" s="146" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B13" s="107" t="s">
         <v>20</v>
@@ -8118,33 +8021,33 @@
     </row>
     <row r="14" spans="1:15" s="127" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="146" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B14" s="107">
-        <v>5000</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="15" spans="1:15" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A15" s="105" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B15" s="105" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="C15" s="43" t="s">
         <v>143</v>
       </c>
       <c r="D15" s="43" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="E15" s="43" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="F15" s="43" t="s">
         <v>144</v>
       </c>
       <c r="G15" s="43" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="H15" s="110" t="s">
         <v>145</v>
@@ -8153,13 +8056,13 @@
         <v>146</v>
       </c>
       <c r="J15" s="147" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="K15" s="147" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="L15" s="147" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="O15" s="180" t="s">
         <v>314</v>
@@ -8182,14 +8085,14 @@
         <v>184</v>
       </c>
       <c r="F16" s="13"/>
-      <c r="G16" s="107" t="s">
-        <v>147</v>
+      <c r="G16" s="107">
+        <v>0.01</v>
       </c>
       <c r="H16" s="13">
-        <v>200000</v>
+        <v>100000</v>
       </c>
       <c r="I16" s="111" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="J16" s="14">
         <v>1E-3</v>
@@ -8201,15 +8104,15 @@
         <v>20</v>
       </c>
       <c r="O16" s="13">
-        <v>50000</v>
-      </c>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" s="127" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="106" t="s">
-        <v>329</v>
+        <v>193</v>
       </c>
       <c r="B17" s="106" t="s">
-        <v>202</v>
+        <v>194</v>
       </c>
       <c r="C17" s="107" t="s">
         <v>149</v>
@@ -8218,19 +8121,21 @@
         <v>183</v>
       </c>
       <c r="E17" s="107" t="s">
-        <v>147</v>
+        <v>184</v>
       </c>
       <c r="F17" s="13"/>
-      <c r="G17" s="107" t="s">
-        <v>147</v>
+      <c r="G17" s="107">
+        <v>0.01</v>
       </c>
       <c r="H17" s="13">
-        <v>100</v>
-      </c>
-      <c r="I17" s="150" t="s">
-        <v>109</v>
-      </c>
-      <c r="J17" s="150"/>
+        <v>50000</v>
+      </c>
+      <c r="I17" s="111" t="s">
+        <v>338</v>
+      </c>
+      <c r="J17" s="14">
+        <v>1E-3</v>
+      </c>
       <c r="K17" s="148" t="s">
         <v>20</v>
       </c>
@@ -8238,15 +8143,15 @@
         <v>20</v>
       </c>
       <c r="O17" s="13">
-        <v>100</v>
+        <v>50000</v>
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A18" s="106" t="s">
-        <v>323</v>
+        <v>191</v>
       </c>
       <c r="B18" s="106" t="s">
-        <v>321</v>
+        <v>188</v>
       </c>
       <c r="C18" s="107" t="s">
         <v>149</v>
@@ -8258,71 +8163,145 @@
         <v>147</v>
       </c>
       <c r="F18" s="13"/>
-      <c r="G18" s="107" t="s">
-        <v>147</v>
+      <c r="G18" s="107">
+        <v>0.01</v>
       </c>
       <c r="H18" s="13">
-        <v>0.02</v>
-      </c>
-      <c r="I18" s="111" t="s">
-        <v>337</v>
-      </c>
-      <c r="J18" s="111"/>
+        <v>200</v>
+      </c>
+      <c r="I18" s="150" t="s">
+        <v>109</v>
+      </c>
+      <c r="J18" s="150"/>
       <c r="K18" s="148" t="s">
-        <v>80</v>
+        <v>20</v>
       </c>
       <c r="L18" s="148" t="s">
         <v>20</v>
       </c>
       <c r="O18" s="13">
-        <v>2.5000000000000001E-2</v>
+        <v>200</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A19" s="19" t="s">
-        <v>185</v>
+      <c r="A19" s="106" t="s">
+        <v>189</v>
       </c>
       <c r="B19" s="106" t="s">
-        <v>186</v>
+        <v>320</v>
       </c>
       <c r="C19" s="107" t="s">
-        <v>187</v>
+        <v>149</v>
       </c>
       <c r="D19" s="107" t="s">
-        <v>178</v>
+        <v>183</v>
       </c>
       <c r="E19" s="107" t="s">
         <v>147</v>
       </c>
       <c r="F19" s="13"/>
-      <c r="G19" s="107" t="s">
+      <c r="G19" s="107">
+        <v>0.01</v>
+      </c>
+      <c r="H19" s="13">
+        <v>0.03</v>
+      </c>
+      <c r="I19" s="111" t="s">
+        <v>338</v>
+      </c>
+      <c r="J19" s="111"/>
+      <c r="K19" s="148" t="s">
+        <v>80</v>
+      </c>
+      <c r="L19" s="148" t="s">
+        <v>20</v>
+      </c>
+      <c r="O19" s="13">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A20" s="106" t="s">
+        <v>190</v>
+      </c>
+      <c r="B20" s="106" t="s">
+        <v>321</v>
+      </c>
+      <c r="C20" s="107" t="s">
+        <v>149</v>
+      </c>
+      <c r="D20" s="107" t="s">
+        <v>183</v>
+      </c>
+      <c r="E20" s="107" t="s">
         <v>147</v>
       </c>
-      <c r="H19" s="13">
-        <v>1000000000</v>
-      </c>
-      <c r="I19" s="111" t="s">
-        <v>337</v>
-      </c>
-      <c r="J19" s="13">
+      <c r="F20" s="13"/>
+      <c r="G20" s="107">
+        <v>0.01</v>
+      </c>
+      <c r="H20" s="13">
+        <v>0.03</v>
+      </c>
+      <c r="I20" s="111" t="s">
+        <v>338</v>
+      </c>
+      <c r="J20" s="20"/>
+      <c r="K20" s="148" t="s">
+        <v>80</v>
+      </c>
+      <c r="L20" s="148" t="s">
+        <v>20</v>
+      </c>
+      <c r="O20" s="13">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A21" s="19" t="s">
+        <v>185</v>
+      </c>
+      <c r="B21" s="106" t="s">
+        <v>186</v>
+      </c>
+      <c r="C21" s="107" t="s">
+        <v>187</v>
+      </c>
+      <c r="D21" s="107" t="s">
+        <v>178</v>
+      </c>
+      <c r="E21" s="107" t="s">
+        <v>147</v>
+      </c>
+      <c r="F21" s="13"/>
+      <c r="G21" s="107">
+        <v>0.99</v>
+      </c>
+      <c r="H21" s="13">
+        <v>2000000000</v>
+      </c>
+      <c r="I21" s="111" t="s">
+        <v>338</v>
+      </c>
+      <c r="J21" s="13">
         <f>0.000000001</f>
         <v>1.0000000000000001E-9</v>
       </c>
-      <c r="K19" s="148" t="s">
-        <v>20</v>
-      </c>
-      <c r="L19" s="148" t="s">
-        <v>20</v>
-      </c>
-      <c r="O19" s="13">
-        <v>50000000</v>
-      </c>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="O20" s="13"/>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="C25" s="128"/>
+      <c r="K21" s="148" t="s">
+        <v>20</v>
+      </c>
+      <c r="L21" s="148" t="s">
+        <v>20</v>
+      </c>
+      <c r="O21" s="13">
+        <v>2000000000</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="O22" s="13"/>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="C27" s="128"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -8332,491 +8311,11 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet20"/>
-  <dimension ref="A1:M17"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="35.625" style="87" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="39.375" style="87" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.75" style="87" customWidth="1"/>
-    <col min="4" max="4" width="10.125" style="87" customWidth="1"/>
-    <col min="5" max="5" width="9" style="87"/>
-    <col min="6" max="6" width="11.625" style="87" customWidth="1"/>
-    <col min="7" max="7" width="19.625" style="87" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.375" style="87" customWidth="1"/>
-    <col min="9" max="9" width="11.25" style="87" customWidth="1"/>
-    <col min="10" max="12" width="9" style="87"/>
-    <col min="13" max="13" width="33.25" style="87" bestFit="1" customWidth="1"/>
-    <col min="14" max="16384" width="9" style="87"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A1" s="159" t="s">
-        <v>203</v>
-      </c>
-      <c r="B1" s="155" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A2" s="154" t="s">
-        <v>204</v>
-      </c>
-      <c r="B2" s="48">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A3" s="108" t="s">
-        <v>195</v>
-      </c>
-      <c r="B3" s="48">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A4" s="154" t="s">
-        <v>205</v>
-      </c>
-      <c r="B4" s="87" t="s">
-        <v>335</v>
-      </c>
-      <c r="C4" s="155" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A5" s="154" t="s">
-        <v>206</v>
-      </c>
-      <c r="C5" s="107"/>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A6" s="106" t="s">
-        <v>215</v>
-      </c>
-      <c r="B6" s="107"/>
-    </row>
-    <row r="7" spans="1:13" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A7" s="151" t="s">
-        <v>196</v>
-      </c>
-      <c r="B7" s="151" t="s">
-        <v>156</v>
-      </c>
-      <c r="C7" s="152" t="s">
-        <v>165</v>
-      </c>
-      <c r="D7" s="152" t="s">
-        <v>167</v>
-      </c>
-      <c r="E7" s="152" t="s">
-        <v>144</v>
-      </c>
-      <c r="F7" s="152" t="s">
-        <v>166</v>
-      </c>
-      <c r="G7" s="152" t="s">
-        <v>146</v>
-      </c>
-      <c r="H7" s="153" t="s">
-        <v>169</v>
-      </c>
-      <c r="I7" s="153" t="s">
-        <v>170</v>
-      </c>
-      <c r="J7" s="153" t="s">
-        <v>171</v>
-      </c>
-      <c r="K7" s="153" t="s">
-        <v>197</v>
-      </c>
-      <c r="L7" s="153" t="s">
-        <v>207</v>
-      </c>
-      <c r="M7" s="153" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A8" s="106" t="s">
-        <v>192</v>
-      </c>
-      <c r="B8" s="106" t="s">
-        <v>148</v>
-      </c>
-      <c r="C8" s="107" t="s">
-        <v>183</v>
-      </c>
-      <c r="D8" s="107" t="s">
-        <v>198</v>
-      </c>
-      <c r="E8" s="152"/>
-      <c r="F8" s="107" t="s">
-        <v>147</v>
-      </c>
-      <c r="G8" s="111" t="s">
-        <v>337</v>
-      </c>
-      <c r="H8" s="14">
-        <v>1E-3</v>
-      </c>
-      <c r="I8" s="148" t="s">
-        <v>20</v>
-      </c>
-      <c r="J8" s="193" t="s">
-        <v>20</v>
-      </c>
-      <c r="K8" s="154" t="s">
-        <v>209</v>
-      </c>
-      <c r="L8" s="153"/>
-      <c r="M8" s="106" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A9" s="154" t="s">
-        <v>213</v>
-      </c>
-      <c r="B9" s="154" t="s">
-        <v>199</v>
-      </c>
-      <c r="C9" s="155" t="s">
-        <v>183</v>
-      </c>
-      <c r="D9" s="155" t="s">
-        <v>198</v>
-      </c>
-      <c r="E9" s="48"/>
-      <c r="F9" s="155" t="s">
-        <v>147</v>
-      </c>
-      <c r="G9" s="145" t="s">
-        <v>337</v>
-      </c>
-      <c r="H9" s="156">
-        <v>1E-3</v>
-      </c>
-      <c r="I9" s="157" t="s">
-        <v>20</v>
-      </c>
-      <c r="J9" s="157" t="s">
-        <v>20</v>
-      </c>
-      <c r="K9" s="154" t="s">
-        <v>209</v>
-      </c>
-      <c r="L9" s="48"/>
-      <c r="M9" s="154" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A10" s="154" t="s">
-        <v>211</v>
-      </c>
-      <c r="B10" s="154" t="s">
-        <v>194</v>
-      </c>
-      <c r="C10" s="155" t="s">
-        <v>183</v>
-      </c>
-      <c r="D10" s="155" t="s">
-        <v>198</v>
-      </c>
-      <c r="E10" s="48"/>
-      <c r="F10" s="155" t="s">
-        <v>147</v>
-      </c>
-      <c r="G10" s="145" t="s">
-        <v>337</v>
-      </c>
-      <c r="H10" s="156">
-        <v>1E-3</v>
-      </c>
-      <c r="I10" s="157" t="s">
-        <v>20</v>
-      </c>
-      <c r="J10" s="157" t="s">
-        <v>20</v>
-      </c>
-      <c r="K10" s="154" t="s">
-        <v>209</v>
-      </c>
-      <c r="L10" s="48"/>
-      <c r="M10" s="154" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A11" s="106" t="s">
-        <v>329</v>
-      </c>
-      <c r="B11" s="106" t="s">
-        <v>202</v>
-      </c>
-      <c r="C11" s="107" t="s">
-        <v>183</v>
-      </c>
-      <c r="D11" s="155" t="s">
-        <v>200</v>
-      </c>
-      <c r="E11" s="152"/>
-      <c r="F11" s="107" t="s">
-        <v>147</v>
-      </c>
-      <c r="G11" s="150" t="s">
-        <v>109</v>
-      </c>
-      <c r="H11" s="150"/>
-      <c r="I11" s="148" t="s">
-        <v>20</v>
-      </c>
-      <c r="J11" s="193" t="s">
-        <v>20</v>
-      </c>
-      <c r="K11" s="154" t="s">
-        <v>209</v>
-      </c>
-      <c r="L11" s="153"/>
-      <c r="M11" s="106" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A12" s="154" t="s">
-        <v>330</v>
-      </c>
-      <c r="B12" s="154" t="s">
-        <v>188</v>
-      </c>
-      <c r="C12" s="155" t="s">
-        <v>183</v>
-      </c>
-      <c r="D12" s="155" t="s">
-        <v>200</v>
-      </c>
-      <c r="E12" s="48"/>
-      <c r="F12" s="155" t="s">
-        <v>147</v>
-      </c>
-      <c r="G12" s="158" t="s">
-        <v>109</v>
-      </c>
-      <c r="H12" s="158"/>
-      <c r="I12" s="157" t="s">
-        <v>20</v>
-      </c>
-      <c r="J12" s="157" t="s">
-        <v>20</v>
-      </c>
-      <c r="K12" s="154" t="s">
-        <v>209</v>
-      </c>
-      <c r="L12" s="48"/>
-      <c r="M12" s="154" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A13" s="154" t="s">
-        <v>331</v>
-      </c>
-      <c r="B13" s="154" t="s">
-        <v>201</v>
-      </c>
-      <c r="C13" s="155" t="s">
-        <v>183</v>
-      </c>
-      <c r="D13" s="155" t="s">
-        <v>200</v>
-      </c>
-      <c r="E13" s="48"/>
-      <c r="F13" s="155" t="s">
-        <v>147</v>
-      </c>
-      <c r="G13" s="158" t="s">
-        <v>109</v>
-      </c>
-      <c r="H13" s="158"/>
-      <c r="I13" s="157" t="s">
-        <v>20</v>
-      </c>
-      <c r="J13" s="157" t="s">
-        <v>20</v>
-      </c>
-      <c r="K13" s="154" t="s">
-        <v>209</v>
-      </c>
-      <c r="L13" s="48"/>
-      <c r="M13" s="154" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A14" s="106" t="s">
-        <v>323</v>
-      </c>
-      <c r="B14" s="106" t="s">
-        <v>321</v>
-      </c>
-      <c r="C14" s="107" t="s">
-        <v>183</v>
-      </c>
-      <c r="D14" s="155" t="s">
-        <v>200</v>
-      </c>
-      <c r="E14" s="152"/>
-      <c r="F14" s="107" t="s">
-        <v>147</v>
-      </c>
-      <c r="G14" s="111" t="s">
-        <v>337</v>
-      </c>
-      <c r="H14" s="111"/>
-      <c r="I14" s="148" t="s">
-        <v>80</v>
-      </c>
-      <c r="J14" s="193" t="s">
-        <v>20</v>
-      </c>
-      <c r="K14" s="154" t="s">
-        <v>209</v>
-      </c>
-      <c r="L14" s="153"/>
-      <c r="M14" s="106" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" s="192" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="106" t="s">
-        <v>324</v>
-      </c>
-      <c r="B15" s="154" t="s">
-        <v>322</v>
-      </c>
-      <c r="C15" s="155" t="s">
-        <v>183</v>
-      </c>
-      <c r="D15" s="155" t="s">
-        <v>200</v>
-      </c>
-      <c r="E15" s="48"/>
-      <c r="F15" s="155" t="s">
-        <v>147</v>
-      </c>
-      <c r="G15" s="145" t="s">
-        <v>337</v>
-      </c>
-      <c r="H15" s="145"/>
-      <c r="I15" s="157" t="s">
-        <v>80</v>
-      </c>
-      <c r="J15" s="157" t="s">
-        <v>20</v>
-      </c>
-      <c r="K15" s="154" t="s">
-        <v>209</v>
-      </c>
-      <c r="L15" s="155" t="s">
-        <v>210</v>
-      </c>
-      <c r="M15" s="106" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" s="141" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="106" t="s">
-        <v>325</v>
-      </c>
-      <c r="B16" s="154" t="s">
-        <v>326</v>
-      </c>
-      <c r="C16" s="155" t="s">
-        <v>183</v>
-      </c>
-      <c r="D16" s="155" t="s">
-        <v>200</v>
-      </c>
-      <c r="E16" s="48"/>
-      <c r="F16" s="155" t="s">
-        <v>147</v>
-      </c>
-      <c r="G16" s="145" t="s">
-        <v>337</v>
-      </c>
-      <c r="H16" s="145"/>
-      <c r="I16" s="148" t="s">
-        <v>80</v>
-      </c>
-      <c r="J16" s="193" t="s">
-        <v>20</v>
-      </c>
-      <c r="K16" s="154" t="s">
-        <v>209</v>
-      </c>
-      <c r="L16" s="153"/>
-      <c r="M16" s="106" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" s="141" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="19" t="s">
-        <v>185</v>
-      </c>
-      <c r="B17" s="106" t="s">
-        <v>186</v>
-      </c>
-      <c r="C17" s="107" t="s">
-        <v>178</v>
-      </c>
-      <c r="D17" s="155" t="s">
-        <v>200</v>
-      </c>
-      <c r="E17" s="152"/>
-      <c r="F17" s="107" t="s">
-        <v>149</v>
-      </c>
-      <c r="G17" s="111" t="s">
-        <v>337</v>
-      </c>
-      <c r="H17" s="13">
-        <f>0.000000001</f>
-        <v>1.0000000000000001E-9</v>
-      </c>
-      <c r="I17" s="148" t="s">
-        <v>20</v>
-      </c>
-      <c r="J17" s="193" t="s">
-        <v>20</v>
-      </c>
-      <c r="K17" s="154" t="s">
-        <v>209</v>
-      </c>
-      <c r="L17" s="153"/>
-      <c r="M17" s="19" t="s">
-        <v>185</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet21"/>
   <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -8827,7 +8326,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="114" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="B1" s="113"/>
     </row>
@@ -9025,11 +8524,10 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet15">
     <tabColor rgb="FFFF0000"/>
@@ -9769,13 +9267,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet23"/>
   <dimension ref="A1:N143"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="H40" sqref="H40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -9801,7 +9299,7 @@
         <v>55</v>
       </c>
       <c r="C2" s="126" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="D2" s="132" t="s">
         <v>109</v>
@@ -11867,16 +11365,14 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet25">
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
   <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -11887,7 +11383,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="44" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="15" x14ac:dyDescent="0.25">
@@ -11898,7 +11394,7 @@
         <v>115</v>
       </c>
       <c r="C2" s="144" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="D2" s="149" t="s">
         <v>179</v>
@@ -12013,22 +11509,22 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C14" s="127"/>
-      <c r="D14" s="189"/>
+      <c r="D14" s="188"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C15" s="128"/>
-      <c r="D15" s="189"/>
+      <c r="D15" s="188"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K52"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A25" workbookViewId="0">
       <selection activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
@@ -12266,7 +11762,7 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="164" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B13" s="155" t="s">
         <v>189</v>
@@ -12283,7 +11779,7 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="165" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B14" s="48">
         <v>1</v>
@@ -12301,7 +11797,7 @@
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" s="165" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B15" s="155" t="s">
         <v>80</v>
@@ -12321,7 +11817,7 @@
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" s="165" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B16" s="155" t="s">
         <v>20</v>
@@ -12401,7 +11897,7 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="164" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B21" s="155" t="s">
         <v>192</v>
@@ -12418,7 +11914,7 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="165" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B22" s="156">
         <v>1E-3</v>
@@ -12435,7 +11931,7 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="165" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B23" s="155" t="s">
         <v>20</v>
@@ -12452,7 +11948,7 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" s="165" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B24" s="155" t="s">
         <v>20</v>
@@ -12529,7 +12025,7 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" s="164" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B29" s="155" t="s">
         <v>191</v>
@@ -12546,7 +12042,7 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" s="165" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B30" s="48">
         <v>1</v>
@@ -12563,7 +12059,7 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" s="165" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B31" s="155" t="s">
         <v>20</v>
@@ -12580,7 +12076,7 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" s="165" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B32" s="155" t="s">
         <v>20</v>
@@ -12669,7 +12165,7 @@
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38" s="164" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B38" s="164"/>
       <c r="C38" s="164"/>
@@ -12679,7 +12175,7 @@
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" s="165" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B39" s="165"/>
       <c r="C39" s="165"/>
@@ -12689,7 +12185,7 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" s="165" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B40" s="165"/>
       <c r="C40" s="165"/>
@@ -12699,7 +12195,7 @@
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41" s="165" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B41" s="165"/>
       <c r="C41" s="165"/>
@@ -12758,7 +12254,7 @@
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A46" s="164" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B46" s="164"/>
       <c r="C46" s="164"/>
@@ -12768,7 +12264,7 @@
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A47" s="165" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B47" s="165"/>
       <c r="C47" s="165"/>
@@ -12778,7 +12274,7 @@
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A48" s="165" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B48" s="165"/>
       <c r="C48" s="165"/>
@@ -12788,7 +12284,7 @@
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" s="165" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B49" s="165"/>
       <c r="C49" s="165"/>
@@ -12839,285 +12335,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet4">
-    <tabColor rgb="FF7030A0"/>
-  </sheetPr>
-  <dimension ref="A1:F25"/>
-  <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="15" style="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="2.875" style="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22" style="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="1.875" style="10" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="9" style="10"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="22" t="s">
-        <v>75</v>
-      </c>
-      <c r="B1" s="10">
-        <v>1</v>
-      </c>
-      <c r="C1" s="21" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="22" t="s">
-        <v>51</v>
-      </c>
-      <c r="D2" s="10">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="22" t="s">
-        <v>50</v>
-      </c>
-      <c r="E3" s="10">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" s="22" t="s">
-        <v>75</v>
-      </c>
-      <c r="B4" s="10">
-        <v>2</v>
-      </c>
-      <c r="C4" s="21" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" s="22" t="s">
-        <v>51</v>
-      </c>
-      <c r="D5" s="10">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" s="22" t="s">
-        <v>50</v>
-      </c>
-      <c r="E6" s="10">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" s="29" t="s">
-        <v>52</v>
-      </c>
-      <c r="B7" s="10">
-        <v>3</v>
-      </c>
-      <c r="C7" s="52" t="s">
-        <v>337</v>
-      </c>
-      <c r="D7" s="29"/>
-      <c r="E7" s="29"/>
-      <c r="F7" s="29"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" s="29" t="s">
-        <v>51</v>
-      </c>
-      <c r="C8" s="29"/>
-      <c r="D8" s="29">
-        <v>5</v>
-      </c>
-      <c r="E8" s="29"/>
-      <c r="F8" s="29"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" s="29" t="s">
-        <v>50</v>
-      </c>
-      <c r="C9" s="29"/>
-      <c r="D9" s="29"/>
-      <c r="E9" s="29">
-        <v>6</v>
-      </c>
-      <c r="F9" s="29"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" s="29" t="s">
-        <v>49</v>
-      </c>
-      <c r="B10" s="10">
-        <v>4</v>
-      </c>
-      <c r="C10" s="30" t="s">
-        <v>318</v>
-      </c>
-      <c r="D10" s="29"/>
-      <c r="E10" s="29"/>
-      <c r="F10" s="29"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" s="29" t="s">
-        <v>49</v>
-      </c>
-      <c r="B11" s="10">
-        <v>5</v>
-      </c>
-      <c r="C11" s="29" t="s">
-        <v>53</v>
-      </c>
-      <c r="D11" s="29"/>
-      <c r="E11" s="29"/>
-      <c r="F11" s="29"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12" s="77" t="s">
-        <v>49</v>
-      </c>
-      <c r="B12" s="10">
-        <v>6</v>
-      </c>
-      <c r="C12" s="77" t="s">
-        <v>78</v>
-      </c>
-      <c r="D12" s="29"/>
-      <c r="E12" s="29"/>
-      <c r="F12" s="29"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13" s="29" t="s">
-        <v>49</v>
-      </c>
-      <c r="B13" s="10">
-        <v>7</v>
-      </c>
-      <c r="C13" s="30" t="s">
-        <v>79</v>
-      </c>
-      <c r="D13" s="29"/>
-      <c r="E13" s="29"/>
-      <c r="F13" s="29"/>
-    </row>
-    <row r="14" spans="1:6" s="94" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="98" t="s">
-        <v>49</v>
-      </c>
-      <c r="B14" s="94">
-        <v>8</v>
-      </c>
-      <c r="C14" s="97" t="s">
-        <v>136</v>
-      </c>
-      <c r="D14" s="98"/>
-      <c r="E14" s="98"/>
-      <c r="F14" s="98"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A15" s="22" t="s">
-        <v>110</v>
-      </c>
-      <c r="B15" s="10">
-        <v>9</v>
-      </c>
-      <c r="C15" s="22" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A16" s="29" t="s">
-        <v>51</v>
-      </c>
-      <c r="C16" s="21"/>
-      <c r="D16" s="10">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A17" s="29" t="s">
-        <v>50</v>
-      </c>
-      <c r="C17" s="21"/>
-      <c r="E17" s="10">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A18" s="22" t="s">
-        <v>110</v>
-      </c>
-      <c r="B18" s="100">
-        <v>10</v>
-      </c>
-      <c r="C18" s="22" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" s="94" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="98" t="s">
-        <v>51</v>
-      </c>
-      <c r="C19" s="22"/>
-      <c r="D19" s="94">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" s="94" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="98" t="s">
-        <v>50</v>
-      </c>
-      <c r="C20" s="22"/>
-      <c r="E20" s="94">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A21" s="22" t="s">
-        <v>110</v>
-      </c>
-      <c r="B21" s="94">
-        <v>11</v>
-      </c>
-      <c r="C21" s="22" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A22" s="98" t="s">
-        <v>51</v>
-      </c>
-      <c r="D22" s="10">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A23" s="98" t="s">
-        <v>50</v>
-      </c>
-      <c r="E23" s="10">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="C24" s="21"/>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A25" s="22"/>
-      <c r="C25" s="21"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet28"/>
   <dimension ref="A1:V51"/>
@@ -13421,19 +12639,19 @@
         <v>300</v>
       </c>
       <c r="B7" s="176" t="s">
-        <v>301</v>
+        <v>334</v>
       </c>
       <c r="C7" s="176" t="s">
-        <v>301</v>
+        <v>334</v>
       </c>
       <c r="D7" s="176" t="s">
-        <v>301</v>
+        <v>334</v>
       </c>
       <c r="E7" s="176" t="s">
-        <v>301</v>
+        <v>334</v>
       </c>
       <c r="F7" s="176" t="s">
-        <v>301</v>
+        <v>334</v>
       </c>
       <c r="H7" s="155" t="s">
         <v>301</v>
@@ -13466,7 +12684,7 @@
         <v>316</v>
       </c>
       <c r="B8" s="161" t="s">
-        <v>317</v>
+        <v>336</v>
       </c>
       <c r="C8" s="161" t="s">
         <v>317</v>
@@ -13497,7 +12715,7 @@
         <v>271</v>
       </c>
       <c r="B9" s="179" t="s">
-        <v>273</v>
+        <v>337</v>
       </c>
       <c r="C9" s="179" t="s">
         <v>273</v>
@@ -13546,7 +12764,7 @@
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A11" s="164" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B11" s="155" t="s">
         <v>192</v>
@@ -13597,7 +12815,7 @@
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A12" s="165" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B12" s="156">
         <v>1E-3</v>
@@ -13648,7 +12866,7 @@
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A13" s="165" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B13" s="155" t="s">
         <v>20</v>
@@ -13699,7 +12917,7 @@
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A14" s="165" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B14" s="155" t="s">
         <v>20</v>
@@ -13845,7 +13063,7 @@
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A18" s="164" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B18" s="155" t="s">
         <v>189</v>
@@ -13896,7 +13114,7 @@
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A19" s="165" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B19" s="48">
         <v>1</v>
@@ -13947,7 +13165,7 @@
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A20" s="165" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B20" s="155" t="s">
         <v>80</v>
@@ -13998,7 +13216,7 @@
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A21" s="165" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B21" s="155" t="s">
         <v>20</v>
@@ -14140,7 +13358,7 @@
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A25" s="164" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B25" s="107" t="s">
         <v>191</v>
@@ -14191,7 +13409,7 @@
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A26" s="165" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B26" s="48">
         <v>1</v>
@@ -14242,7 +13460,7 @@
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A27" s="165" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B27" s="48" t="s">
         <v>20</v>
@@ -14293,7 +13511,7 @@
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A28" s="165" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B28" s="48" t="s">
         <v>20</v>
@@ -14376,7 +13594,7 @@
         <v>222</v>
       </c>
       <c r="B30" s="155" t="s">
-        <v>298</v>
+        <v>335</v>
       </c>
       <c r="C30" s="155" t="s">
         <v>298</v>
@@ -14439,7 +13657,7 @@
     </row>
     <row r="32" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A32" s="164" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B32" s="107" t="s">
         <v>190</v>
@@ -14490,7 +13708,7 @@
     </row>
     <row r="33" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A33" s="165" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B33" s="48">
         <v>1</v>
@@ -14541,7 +13759,7 @@
     </row>
     <row r="34" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A34" s="165" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B34" s="48" t="s">
         <v>80</v>
@@ -14592,7 +13810,7 @@
     </row>
     <row r="35" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A35" s="165" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B35" s="48" t="s">
         <v>20</v>
@@ -14742,7 +13960,7 @@
     </row>
     <row r="39" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A39" s="164" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B39" s="107" t="s">
         <v>193</v>
@@ -14793,7 +14011,7 @@
     </row>
     <row r="40" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A40" s="165" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B40" s="156">
         <v>1E-3</v>
@@ -14844,7 +14062,7 @@
     </row>
     <row r="41" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A41" s="165" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B41" s="48" t="s">
         <v>20</v>
@@ -14895,7 +14113,7 @@
     </row>
     <row r="42" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A42" s="165" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B42" s="48" t="s">
         <v>20</v>
@@ -15042,7 +14260,7 @@
     </row>
     <row r="46" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A46" s="164" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B46" s="148" t="s">
         <v>185</v>
@@ -15093,7 +14311,7 @@
     </row>
     <row r="47" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A47" s="165" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B47" s="13">
         <f>0.000000001</f>
@@ -15159,7 +14377,7 @@
     </row>
     <row r="48" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A48" s="165" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B48" s="155" t="s">
         <v>20</v>
@@ -15210,7 +14428,7 @@
     </row>
     <row r="49" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A49" s="165" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B49" s="155" t="s">
         <v>20</v>
@@ -15337,12 +14555,290 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet4">
+    <tabColor rgb="FF7030A0"/>
+  </sheetPr>
+  <dimension ref="A1:F25"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="15" style="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="2.875" style="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22" style="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="1.875" style="10" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9" style="10"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" s="22" t="s">
+        <v>75</v>
+      </c>
+      <c r="B1" s="10">
+        <v>1</v>
+      </c>
+      <c r="C1" s="21" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="D2" s="10">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="22" t="s">
+        <v>50</v>
+      </c>
+      <c r="E3" s="10">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="22" t="s">
+        <v>75</v>
+      </c>
+      <c r="B4" s="10">
+        <v>2</v>
+      </c>
+      <c r="C4" s="21" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="D5" s="10">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" s="22" t="s">
+        <v>50</v>
+      </c>
+      <c r="E6" s="10">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" s="29" t="s">
+        <v>52</v>
+      </c>
+      <c r="B7" s="10">
+        <v>3</v>
+      </c>
+      <c r="C7" s="52" t="s">
+        <v>338</v>
+      </c>
+      <c r="D7" s="29"/>
+      <c r="E7" s="29"/>
+      <c r="F7" s="29"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" s="29" t="s">
+        <v>51</v>
+      </c>
+      <c r="C8" s="29"/>
+      <c r="D8" s="29">
+        <v>5</v>
+      </c>
+      <c r="E8" s="29"/>
+      <c r="F8" s="29"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" s="29" t="s">
+        <v>50</v>
+      </c>
+      <c r="C9" s="29"/>
+      <c r="D9" s="29"/>
+      <c r="E9" s="29">
+        <v>6</v>
+      </c>
+      <c r="F9" s="29"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" s="29" t="s">
+        <v>49</v>
+      </c>
+      <c r="B10" s="10">
+        <v>4</v>
+      </c>
+      <c r="C10" s="30" t="s">
+        <v>318</v>
+      </c>
+      <c r="D10" s="29"/>
+      <c r="E10" s="29"/>
+      <c r="F10" s="29"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" s="29" t="s">
+        <v>49</v>
+      </c>
+      <c r="B11" s="10">
+        <v>5</v>
+      </c>
+      <c r="C11" s="29" t="s">
+        <v>53</v>
+      </c>
+      <c r="D11" s="29"/>
+      <c r="E11" s="29"/>
+      <c r="F11" s="29"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" s="77" t="s">
+        <v>49</v>
+      </c>
+      <c r="B12" s="10">
+        <v>6</v>
+      </c>
+      <c r="C12" s="77" t="s">
+        <v>78</v>
+      </c>
+      <c r="D12" s="29"/>
+      <c r="E12" s="29"/>
+      <c r="F12" s="29"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" s="29" t="s">
+        <v>49</v>
+      </c>
+      <c r="B13" s="10">
+        <v>7</v>
+      </c>
+      <c r="C13" s="30" t="s">
+        <v>79</v>
+      </c>
+      <c r="D13" s="29"/>
+      <c r="E13" s="29"/>
+      <c r="F13" s="29"/>
+    </row>
+    <row r="14" spans="1:6" s="94" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="98" t="s">
+        <v>49</v>
+      </c>
+      <c r="B14" s="94">
+        <v>8</v>
+      </c>
+      <c r="C14" s="97" t="s">
+        <v>136</v>
+      </c>
+      <c r="D14" s="98"/>
+      <c r="E14" s="98"/>
+      <c r="F14" s="98"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" s="22" t="s">
+        <v>110</v>
+      </c>
+      <c r="B15" s="10">
+        <v>9</v>
+      </c>
+      <c r="C15" s="22" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" s="29" t="s">
+        <v>51</v>
+      </c>
+      <c r="C16" s="21"/>
+      <c r="D16" s="10">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" s="29" t="s">
+        <v>50</v>
+      </c>
+      <c r="C17" s="21"/>
+      <c r="E17" s="10">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" s="22" t="s">
+        <v>110</v>
+      </c>
+      <c r="B18" s="100">
+        <v>10</v>
+      </c>
+      <c r="C18" s="22" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" s="94" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="98" t="s">
+        <v>51</v>
+      </c>
+      <c r="C19" s="22"/>
+      <c r="D19" s="94">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" s="94" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="98" t="s">
+        <v>50</v>
+      </c>
+      <c r="C20" s="22"/>
+      <c r="E20" s="94">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21" s="22" t="s">
+        <v>110</v>
+      </c>
+      <c r="B21" s="94">
+        <v>11</v>
+      </c>
+      <c r="C21" s="22" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22" s="98" t="s">
+        <v>51</v>
+      </c>
+      <c r="D22" s="10">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23" s="98" t="s">
+        <v>50</v>
+      </c>
+      <c r="E23" s="10">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C24" s="21"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25" s="22"/>
+      <c r="C25" s="21"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D39" sqref="D39"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -15363,7 +14859,7 @@
         <v>126</v>
       </c>
       <c r="B2" s="87" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -15376,6 +14872,485 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="35.625" style="87" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="39.375" style="87" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.75" style="87" customWidth="1"/>
+    <col min="4" max="4" width="10.125" style="87" customWidth="1"/>
+    <col min="5" max="5" width="9" style="87"/>
+    <col min="6" max="6" width="11.625" style="87" customWidth="1"/>
+    <col min="7" max="7" width="19.625" style="87" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.375" style="87" customWidth="1"/>
+    <col min="9" max="9" width="11.25" style="87" customWidth="1"/>
+    <col min="10" max="12" width="9" style="87"/>
+    <col min="13" max="13" width="33.25" style="87" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="9" style="87"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A1" s="159" t="s">
+        <v>203</v>
+      </c>
+      <c r="B1" s="155" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A2" s="154" t="s">
+        <v>204</v>
+      </c>
+      <c r="B2" s="48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A3" s="108" t="s">
+        <v>195</v>
+      </c>
+      <c r="B3" s="48">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A4" s="154" t="s">
+        <v>205</v>
+      </c>
+      <c r="B4" s="87" t="s">
+        <v>341</v>
+      </c>
+      <c r="C4" s="155" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A5" s="154" t="s">
+        <v>206</v>
+      </c>
+      <c r="C5" s="107"/>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A6" s="106" t="s">
+        <v>215</v>
+      </c>
+      <c r="B6" s="107"/>
+    </row>
+    <row r="7" spans="1:13" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A7" s="151" t="s">
+        <v>196</v>
+      </c>
+      <c r="B7" s="151" t="s">
+        <v>157</v>
+      </c>
+      <c r="C7" s="152" t="s">
+        <v>166</v>
+      </c>
+      <c r="D7" s="152" t="s">
+        <v>168</v>
+      </c>
+      <c r="E7" s="152" t="s">
+        <v>144</v>
+      </c>
+      <c r="F7" s="152" t="s">
+        <v>167</v>
+      </c>
+      <c r="G7" s="152" t="s">
+        <v>146</v>
+      </c>
+      <c r="H7" s="153" t="s">
+        <v>170</v>
+      </c>
+      <c r="I7" s="153" t="s">
+        <v>171</v>
+      </c>
+      <c r="J7" s="153" t="s">
+        <v>172</v>
+      </c>
+      <c r="K7" s="153" t="s">
+        <v>197</v>
+      </c>
+      <c r="L7" s="153" t="s">
+        <v>207</v>
+      </c>
+      <c r="M7" s="153" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A8" s="106" t="s">
+        <v>192</v>
+      </c>
+      <c r="B8" s="106" t="s">
+        <v>148</v>
+      </c>
+      <c r="C8" s="107" t="s">
+        <v>183</v>
+      </c>
+      <c r="D8" s="107" t="s">
+        <v>198</v>
+      </c>
+      <c r="E8" s="152"/>
+      <c r="F8" s="107" t="s">
+        <v>147</v>
+      </c>
+      <c r="G8" s="111" t="s">
+        <v>338</v>
+      </c>
+      <c r="H8" s="14">
+        <v>1E-3</v>
+      </c>
+      <c r="I8" s="148" t="s">
+        <v>20</v>
+      </c>
+      <c r="J8" s="192" t="s">
+        <v>20</v>
+      </c>
+      <c r="K8" s="154" t="s">
+        <v>209</v>
+      </c>
+      <c r="L8" s="153"/>
+      <c r="M8" s="106" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A9" s="154" t="s">
+        <v>213</v>
+      </c>
+      <c r="B9" s="154" t="s">
+        <v>199</v>
+      </c>
+      <c r="C9" s="155" t="s">
+        <v>183</v>
+      </c>
+      <c r="D9" s="155" t="s">
+        <v>198</v>
+      </c>
+      <c r="E9" s="48"/>
+      <c r="F9" s="155" t="s">
+        <v>147</v>
+      </c>
+      <c r="G9" s="145" t="s">
+        <v>338</v>
+      </c>
+      <c r="H9" s="156">
+        <v>1E-3</v>
+      </c>
+      <c r="I9" s="157" t="s">
+        <v>20</v>
+      </c>
+      <c r="J9" s="157" t="s">
+        <v>20</v>
+      </c>
+      <c r="K9" s="154" t="s">
+        <v>209</v>
+      </c>
+      <c r="L9" s="48"/>
+      <c r="M9" s="154" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A10" s="154" t="s">
+        <v>211</v>
+      </c>
+      <c r="B10" s="154" t="s">
+        <v>194</v>
+      </c>
+      <c r="C10" s="155" t="s">
+        <v>183</v>
+      </c>
+      <c r="D10" s="155" t="s">
+        <v>198</v>
+      </c>
+      <c r="E10" s="48"/>
+      <c r="F10" s="155" t="s">
+        <v>147</v>
+      </c>
+      <c r="G10" s="145" t="s">
+        <v>338</v>
+      </c>
+      <c r="H10" s="156">
+        <v>1E-3</v>
+      </c>
+      <c r="I10" s="157" t="s">
+        <v>20</v>
+      </c>
+      <c r="J10" s="157" t="s">
+        <v>20</v>
+      </c>
+      <c r="K10" s="154" t="s">
+        <v>209</v>
+      </c>
+      <c r="L10" s="48"/>
+      <c r="M10" s="154" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A11" s="106" t="s">
+        <v>323</v>
+      </c>
+      <c r="B11" s="106" t="s">
+        <v>202</v>
+      </c>
+      <c r="C11" s="107" t="s">
+        <v>183</v>
+      </c>
+      <c r="D11" s="155" t="s">
+        <v>200</v>
+      </c>
+      <c r="E11" s="152"/>
+      <c r="F11" s="107" t="s">
+        <v>147</v>
+      </c>
+      <c r="G11" s="150" t="s">
+        <v>109</v>
+      </c>
+      <c r="H11" s="150"/>
+      <c r="I11" s="148" t="s">
+        <v>20</v>
+      </c>
+      <c r="J11" s="192" t="s">
+        <v>20</v>
+      </c>
+      <c r="K11" s="154" t="s">
+        <v>209</v>
+      </c>
+      <c r="L11" s="153"/>
+      <c r="M11" s="106" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A12" s="154" t="s">
+        <v>324</v>
+      </c>
+      <c r="B12" s="154" t="s">
+        <v>188</v>
+      </c>
+      <c r="C12" s="155" t="s">
+        <v>183</v>
+      </c>
+      <c r="D12" s="155" t="s">
+        <v>200</v>
+      </c>
+      <c r="E12" s="48"/>
+      <c r="F12" s="155" t="s">
+        <v>147</v>
+      </c>
+      <c r="G12" s="158" t="s">
+        <v>109</v>
+      </c>
+      <c r="H12" s="158"/>
+      <c r="I12" s="157" t="s">
+        <v>20</v>
+      </c>
+      <c r="J12" s="157" t="s">
+        <v>20</v>
+      </c>
+      <c r="K12" s="154" t="s">
+        <v>209</v>
+      </c>
+      <c r="L12" s="48"/>
+      <c r="M12" s="154" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A13" s="154" t="s">
+        <v>326</v>
+      </c>
+      <c r="B13" s="154" t="s">
+        <v>201</v>
+      </c>
+      <c r="C13" s="155" t="s">
+        <v>183</v>
+      </c>
+      <c r="D13" s="155" t="s">
+        <v>200</v>
+      </c>
+      <c r="E13" s="48"/>
+      <c r="F13" s="155" t="s">
+        <v>147</v>
+      </c>
+      <c r="G13" s="158" t="s">
+        <v>109</v>
+      </c>
+      <c r="H13" s="158"/>
+      <c r="I13" s="157" t="s">
+        <v>20</v>
+      </c>
+      <c r="J13" s="157" t="s">
+        <v>20</v>
+      </c>
+      <c r="K13" s="154" t="s">
+        <v>209</v>
+      </c>
+      <c r="L13" s="48"/>
+      <c r="M13" s="154" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A14" s="106" t="s">
+        <v>328</v>
+      </c>
+      <c r="B14" s="106" t="s">
+        <v>329</v>
+      </c>
+      <c r="C14" s="107" t="s">
+        <v>183</v>
+      </c>
+      <c r="D14" s="155" t="s">
+        <v>200</v>
+      </c>
+      <c r="E14" s="152"/>
+      <c r="F14" s="107" t="s">
+        <v>147</v>
+      </c>
+      <c r="G14" s="111" t="s">
+        <v>338</v>
+      </c>
+      <c r="H14" s="111"/>
+      <c r="I14" s="148" t="s">
+        <v>80</v>
+      </c>
+      <c r="J14" s="192" t="s">
+        <v>20</v>
+      </c>
+      <c r="K14" s="154" t="s">
+        <v>209</v>
+      </c>
+      <c r="L14" s="153"/>
+      <c r="M14" s="106" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" s="193" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="106" t="s">
+        <v>330</v>
+      </c>
+      <c r="B15" s="154" t="s">
+        <v>320</v>
+      </c>
+      <c r="C15" s="155" t="s">
+        <v>183</v>
+      </c>
+      <c r="D15" s="155" t="s">
+        <v>200</v>
+      </c>
+      <c r="E15" s="48"/>
+      <c r="F15" s="155" t="s">
+        <v>147</v>
+      </c>
+      <c r="G15" s="145" t="s">
+        <v>338</v>
+      </c>
+      <c r="H15" s="145"/>
+      <c r="I15" s="157" t="s">
+        <v>80</v>
+      </c>
+      <c r="J15" s="157" t="s">
+        <v>20</v>
+      </c>
+      <c r="K15" s="154" t="s">
+        <v>209</v>
+      </c>
+      <c r="L15" s="155" t="s">
+        <v>210</v>
+      </c>
+      <c r="M15" s="106" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" s="141" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="106" t="s">
+        <v>332</v>
+      </c>
+      <c r="B16" s="154" t="s">
+        <v>321</v>
+      </c>
+      <c r="C16" s="155" t="s">
+        <v>183</v>
+      </c>
+      <c r="D16" s="155" t="s">
+        <v>200</v>
+      </c>
+      <c r="E16" s="48"/>
+      <c r="F16" s="155" t="s">
+        <v>147</v>
+      </c>
+      <c r="G16" s="145" t="s">
+        <v>338</v>
+      </c>
+      <c r="H16" s="145"/>
+      <c r="I16" s="148" t="s">
+        <v>80</v>
+      </c>
+      <c r="J16" s="192" t="s">
+        <v>20</v>
+      </c>
+      <c r="K16" s="154" t="s">
+        <v>209</v>
+      </c>
+      <c r="L16" s="153"/>
+      <c r="M16" s="106" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" s="141" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="19" t="s">
+        <v>185</v>
+      </c>
+      <c r="B17" s="106" t="s">
+        <v>186</v>
+      </c>
+      <c r="C17" s="107" t="s">
+        <v>178</v>
+      </c>
+      <c r="D17" s="155" t="s">
+        <v>200</v>
+      </c>
+      <c r="E17" s="152"/>
+      <c r="F17" s="107" t="s">
+        <v>149</v>
+      </c>
+      <c r="G17" s="111" t="s">
+        <v>338</v>
+      </c>
+      <c r="H17" s="13">
+        <f>0.000000001</f>
+        <v>1.0000000000000001E-9</v>
+      </c>
+      <c r="I17" s="148" t="s">
+        <v>20</v>
+      </c>
+      <c r="J17" s="192" t="s">
+        <v>20</v>
+      </c>
+      <c r="K17" s="154" t="s">
+        <v>209</v>
+      </c>
+      <c r="L17" s="153"/>
+      <c r="M17" s="19" t="s">
+        <v>185</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -15387,7 +15362,7 @@
   <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15422,7 +15397,7 @@
       <c r="J1" s="72"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="191" t="s">
+      <c r="A2" s="189" t="s">
         <v>318</v>
       </c>
       <c r="B2" s="42">
@@ -15430,7 +15405,7 @@
         <v>76800000000</v>
       </c>
       <c r="C2" s="190">
-        <v>3.595022937357871E-7</v>
+        <v>3.5950229373578699E-7</v>
       </c>
       <c r="D2" s="107">
         <v>1.2759</v>
@@ -15460,7 +15435,7 @@
   </sheetPr>
   <dimension ref="A1:U5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="I1" workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
@@ -15636,7 +15611,7 @@
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A5" s="18" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="B5" s="13">
         <v>2.0000000000000002E-5</v>
@@ -15696,7 +15671,7 @@
   <sheetData>
     <row r="1" spans="1:4" s="5" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="44" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -16186,7 +16161,7 @@
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="18" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="B2" s="13">
         <v>130.19999999999999</v>
@@ -16243,9 +16218,7 @@
   </sheetPr>
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -16254,7 +16227,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="89" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -16375,9 +16348,9 @@
   </sheetPr>
   <dimension ref="A1:Y103"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="J1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="N7" sqref="N7"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" topLeftCell="L1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16474,15 +16447,15 @@
         <v>106</v>
       </c>
       <c r="X1" s="56" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="Y1" s="56" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A2" s="58" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="B2" s="59">
         <v>39</v>
@@ -16502,8 +16475,8 @@
       <c r="G2" s="61" t="s">
         <v>36</v>
       </c>
-      <c r="H2" s="188" t="s">
-        <v>320</v>
+      <c r="H2" s="191" t="s">
+        <v>322</v>
       </c>
       <c r="I2" s="62"/>
       <c r="K2" s="59">
@@ -16516,7 +16489,7 @@
         <v>30000</v>
       </c>
       <c r="N2" s="70" t="s">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="O2" s="59" t="s">
         <v>20</v>
@@ -17708,8 +17681,8 @@
   </sheetPr>
   <dimension ref="A1:P10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -17735,7 +17708,7 @@
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" s="87" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="B1" s="87"/>
       <c r="C1" s="87"/>
@@ -17787,16 +17760,16 @@
         <v>45</v>
       </c>
       <c r="M2" s="34" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="N2" s="34" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="O2" s="34" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="P2" s="34" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.2">

</xml_diff>